<commit_message>
4.3.6. Adding hotkeys checking
</commit_message>
<xml_diff>
--- a/tests/manual/integration/4.3.6.ConfiguratorMSHK-01.WardrobeDepth.InputField.xlsx
+++ b/tests/manual/integration/4.3.6.ConfiguratorMSHK-01.WardrobeDepth.InputField.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\art\tests\manual\integration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pa\art\tests\manual\integration\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9C7DF2-D670-42FC-AB36-43E787AD0466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>Модуль</t>
   </si>
@@ -87,18 +88,99 @@
     <t>1. Нажать функциональную клавишу F12</t>
   </si>
   <si>
-    <t>Открылось окно инструментов разработки
-браузера</t>
-  </si>
-  <si>
     <t>В консоли инструментов разработчика
 отсутствуют сообщения об ошибках</t>
+  </si>
+  <si>
+    <t>Открылось окно инструментов разработчика в браузере</t>
+  </si>
+  <si>
+    <t>1. Нажимать клавишу Tab до установки фокуса на поле ввода "Глубина шкафа"</t>
+  </si>
+  <si>
+    <t>2. Нажать клавишу Backspace</t>
+  </si>
+  <si>
+    <t>3. В поле ввода "Глубина шкафа" ввести
+цифру "4"</t>
+  </si>
+  <si>
+    <t>4. Нажать клавишу "стрелка вниз" 4 раза</t>
+  </si>
+  <si>
+    <t>Фокус поочередно устанавливается на
+опции "430", "470"</t>
+  </si>
+  <si>
+    <t>5. Нажать клавишу "стрелка вверх" 4 раза</t>
+  </si>
+  <si>
+    <t>6. Нажать клавишу Esc</t>
+  </si>
+  <si>
+    <t>7. В поле ввода "Глубина шкафа" ввести
+цифру "3"</t>
+  </si>
+  <si>
+    <t>Фокус установлен на опцию "430"</t>
+  </si>
+  <si>
+    <t>8. Нажать клавишу "стрелка вниз" 1 раз</t>
+  </si>
+  <si>
+    <t>9. Нажать клавишу Enter</t>
+  </si>
+  <si>
+    <t>В поле ввода "Глубина шкафа" установлено значение "430", Datalist отсутствует</t>
+  </si>
+  <si>
+    <t>В поле ввода "Глубина шкафа" установлено
+значение "43", под полем ввода находится Datalist с опцией "430"</t>
+  </si>
+  <si>
+    <t>В поле ввода "Глубина шкафа" установлено
+значение "4", Datalist отсутствует</t>
+  </si>
+  <si>
+    <t>В поле ввода "Глубина шкафа" установлено
+значение "4", под полем ввода появился Datalist с опциями "430", "470"</t>
+  </si>
+  <si>
+    <t>Фокус установлен на поле ввода "Глубина шкафа", значение в поле ввода отсутствует, курсор в начале поля ввода</t>
+  </si>
+  <si>
+    <t>Фокус установлен на поле ввода "Глубина шкафа", значение поля по умолчанию "430" выделено автоматически</t>
+  </si>
+  <si>
+    <t>10. ЛКМ установить выделение значения
+"430" поля ввода "Глубина шкафа"</t>
+  </si>
+  <si>
+    <t>Установлено выделение значения
+"430" поля ввода "Глубина шкафа"</t>
+  </si>
+  <si>
+    <t>11. Нажать сочетание клавиш Ctrl+C</t>
+  </si>
+  <si>
+    <t>12. Нажать клавишу Backspace</t>
+  </si>
+  <si>
+    <t>В поле ввода "Глубина шкафа" установлено
+значение "430", под полем ввода находится Datalist с опцией "430"</t>
+  </si>
+  <si>
+    <t>Работа клавиш Tab, Enter, Esc,
+стрелка вверх, стрелка вниз, Ctrl+C, Ctrl+V</t>
+  </si>
+  <si>
+    <t>13. Нажать сочетание клавиш Ctrl+V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -143,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -152,25 +234,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -489,12 +565,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4:C5"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -503,8 +579,8 @@
     <col min="2" max="2" width="23.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="34.88671875" style="1" customWidth="1"/>
     <col min="4" max="4" width="39.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="43.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="42.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="45" style="1" customWidth="1"/>
+    <col min="6" max="6" width="46.109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" style="1" customWidth="1"/>
     <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -533,74 +609,245 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="6"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="8" t="s">
+      <c r="A3" s="6"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="6"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" s="3" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9">
+      <c r="A4" s="6">
         <v>2</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>19</v>
-      </c>
+    </row>
+    <row r="6" spans="1:7" s="3" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="3" customFormat="1" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="3" customFormat="1" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="3" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="3" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="3" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="3" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="3" customFormat="1" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="12">
+    <mergeCell ref="A6:A18"/>
+    <mergeCell ref="B6:B18"/>
+    <mergeCell ref="C6:C18"/>
+    <mergeCell ref="D6:D18"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>

</xml_diff>

<commit_message>
A variant of the test cases 4.3.6, 4.3.15 in one file has been completed
</commit_message>
<xml_diff>
--- a/tests/manual/integration/4.3.6.ConfiguratorMSHK-01.WardrobeDepth.InputField.xlsx
+++ b/tests/manual/integration/4.3.6.ConfiguratorMSHK-01.WardrobeDepth.InputField.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pa\art\tests\manual\integration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F465094F-1167-4BD6-BF34-1C299350EB99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE2D16B-2612-45D0-B9D3-ECCD997C26AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="111">
   <si>
     <t>Модуль</t>
   </si>
@@ -739,6 +739,175 @@
       <t>"
 4. Таблица раздельной выписки и
 кнопка "Скачать Excel" видимы.</t>
+    </r>
+  </si>
+  <si>
+    <t>В поле ввода "Глубина шкафа" установлено
+значение "Не особенно длинная строка", начало строки выходит за пределы поля ввода.</t>
+  </si>
+  <si>
+    <t>1. В поле ввода "Глубина шкафа" ввести
+значение "Не особенно длинная строка"</t>
+  </si>
+  <si>
+    <r>
+      <t>1. В поле ввода "Глубина шкафа" установлено
+значение "Не особенно длинная строка" красного цвета.
+2. Фокус установлен на поле ввода "Ширина спального места"
+3. В области уведомлений появился текст красного цвета "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Укажите глубину шкафа не менее глубины механизма и не более 600 мм.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"
+4. Таблица раздельной выписки и
+кнопка "Скачать Excel" скрыты.</t>
+    </r>
+  </si>
+  <si>
+    <t>Ввод спецсимволов</t>
+  </si>
+  <si>
+    <t>1. В поле ввода "Глубина шкафа" ввести
+значение "@$%&amp;*"</t>
+  </si>
+  <si>
+    <t>В поле ввода "Глубина шкафа" установлено
+значение "@$%&amp;*".</t>
+  </si>
+  <si>
+    <r>
+      <t>1. В поле ввода "Глубина шкафа" установлено
+значение "@$%&amp;*" красного цвета.
+2. Фокус установлен на поле ввода "Ширина спального места"
+3. В области уведомлений появился текст красного цвета "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Укажите глубину шкафа не менее глубины механизма и не более 600 мм.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"
+4. Таблица раздельной выписки и
+кнопка "Скачать Excel" скрыты.</t>
+    </r>
+  </si>
+  <si>
+    <t>Ввод текста</t>
+  </si>
+  <si>
+    <t>Ввод пробела</t>
+  </si>
+  <si>
+    <t>1. В поле ввода "Глубина шкафа" ввести
+значение одинарный пробел " "</t>
+  </si>
+  <si>
+    <t>В поле ввода "Глубина шкафа" установлено
+значение одинарный пробел " ".</t>
+  </si>
+  <si>
+    <r>
+      <t>1. В поле ввода "Глубина шкафа" установлено
+значение одинарный пробел " ".
+2. Фокус установлен на поле ввода "Ширина спального места"
+3. В области уведомлений появился текст красного цвета "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Укажите глубину шкафа не менее глубины механизма и не более 600 мм.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"
+4. Таблица раздельной выписки и
+кнопка "Скачать Excel" скрыты.</t>
+    </r>
+  </si>
+  <si>
+    <t>Ввод пустого поля</t>
+  </si>
+  <si>
+    <t>1. Очистить значение поля ввода "Глубина шкафа"</t>
+  </si>
+  <si>
+    <t>В поле ввода "Глубина шкафа" пустое.</t>
+  </si>
+  <si>
+    <r>
+      <t>1. В поле ввода "Глубина шкафа" пустое.
+2. Фокус установлен на поле ввода "Ширина спального места"
+3. В области уведомлений появился текст красного цвета "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Укажите глубину шкафа не менее глубины механизма и не более 600 мм.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"
+4. Таблица раздельной выписки и
+кнопка "Скачать Excel" скрыты.</t>
     </r>
   </si>
 </sst>
@@ -818,7 +987,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -829,20 +998,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1158,11 +1336,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G53" sqref="G53"/>
+      <selection pane="bottomLeft" activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1201,16 +1379,16 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -1224,10 +1402,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
       <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
@@ -1237,16 +1415,16 @@
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
+      <c r="A4" s="6">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -1260,10 +1438,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="5"/>
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="6"/>
       <c r="E5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1273,16 +1451,16 @@
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="A6" s="6">
         <v>3</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="3" t="s">
@@ -1296,10 +1474,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="5"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="3" t="s">
         <v>20</v>
       </c>
@@ -1309,10 +1487,10 @@
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="5"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="6"/>
       <c r="E8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1322,10 +1500,10 @@
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="5"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="2" t="s">
         <v>22</v>
       </c>
@@ -1335,10 +1513,10 @@
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="5"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="6"/>
       <c r="E10" s="2" t="s">
         <v>24</v>
       </c>
@@ -1348,10 +1526,10 @@
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="5"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="6"/>
       <c r="E11" s="2" t="s">
         <v>25</v>
       </c>
@@ -1361,10 +1539,10 @@
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="5"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="6"/>
       <c r="E12" s="3" t="s">
         <v>26</v>
       </c>
@@ -1374,10 +1552,10 @@
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="5"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="6"/>
       <c r="E13" s="2" t="s">
         <v>28</v>
       </c>
@@ -1387,10 +1565,10 @@
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="5"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="6"/>
       <c r="E14" s="2" t="s">
         <v>29</v>
       </c>
@@ -1400,10 +1578,10 @@
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="5"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="6"/>
       <c r="E15" s="3" t="s">
         <v>36</v>
       </c>
@@ -1413,10 +1591,10 @@
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="5"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="6"/>
       <c r="E16" s="2" t="s">
         <v>38</v>
       </c>
@@ -1426,10 +1604,10 @@
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="5"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="6"/>
       <c r="E17" s="3" t="s">
         <v>39</v>
       </c>
@@ -1439,10 +1617,10 @@
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="5"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="6"/>
       <c r="E18" s="2" t="s">
         <v>42</v>
       </c>
@@ -1452,16 +1630,16 @@
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
+      <c r="A19" s="6">
         <v>4</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="3" t="s">
@@ -1475,10 +1653,10 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="157.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="5"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="6"/>
       <c r="E20" s="2" t="s">
         <v>11</v>
       </c>
@@ -1488,16 +1666,16 @@
       <c r="G20" s="8"/>
     </row>
     <row r="21" spans="1:7" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
+      <c r="A21" s="6">
         <v>5</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="3" t="s">
@@ -1511,10 +1689,10 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
       <c r="E22" s="2" t="s">
         <v>11</v>
       </c>
@@ -1524,16 +1702,16 @@
       <c r="G22" s="8"/>
     </row>
     <row r="23" spans="1:7" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
+      <c r="A23" s="6">
         <v>6</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="3" t="s">
@@ -1547,10 +1725,10 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="158.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="5"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="6"/>
       <c r="E24" s="2" t="s">
         <v>11</v>
       </c>
@@ -1560,10 +1738,10 @@
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="5"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="6"/>
       <c r="E25" s="3" t="s">
         <v>58</v>
       </c>
@@ -1573,10 +1751,10 @@
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" ht="132" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="5"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="6"/>
       <c r="E26" s="2" t="s">
         <v>61</v>
       </c>
@@ -1586,10 +1764,10 @@
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="5"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="6"/>
       <c r="E27" s="3" t="s">
         <v>62</v>
       </c>
@@ -1599,10 +1777,10 @@
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" ht="160.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="5"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="6"/>
       <c r="E28" s="2" t="s">
         <v>65</v>
       </c>
@@ -1612,16 +1790,16 @@
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="5">
+      <c r="A29" s="6">
         <v>7</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="4" t="s">
         <v>67</v>
       </c>
       <c r="E29" s="3" t="s">
@@ -1630,106 +1808,106 @@
       <c r="F29" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="G29" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="171.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="5"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="6"/>
+      <c r="A30" s="6"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="4"/>
       <c r="E30" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G30" s="4"/>
+      <c r="G30" s="5"/>
     </row>
     <row r="31" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A31" s="5"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="6"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="4"/>
       <c r="E31" s="3" t="s">
         <v>71</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="G31" s="4"/>
+      <c r="G31" s="5"/>
     </row>
     <row r="32" spans="1:7" ht="140.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="5"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="6"/>
+      <c r="A32" s="6"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="4"/>
       <c r="E32" s="2" t="s">
         <v>61</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="G32" s="4"/>
+      <c r="G32" s="5"/>
     </row>
     <row r="33" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="5"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="6"/>
+      <c r="A33" s="6"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="4"/>
       <c r="E33" s="3" t="s">
         <v>75</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G33" s="4"/>
+      <c r="G33" s="5"/>
     </row>
     <row r="34" spans="1:7" ht="135.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="6"/>
+      <c r="A34" s="6"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="4"/>
       <c r="E34" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="G34" s="4"/>
+      <c r="G34" s="5"/>
     </row>
     <row r="35" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A35" s="5"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="6"/>
+      <c r="A35" s="6"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="4"/>
       <c r="E35" s="3" t="s">
         <v>77</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G35" s="4"/>
+      <c r="G35" s="5"/>
     </row>
     <row r="36" spans="1:7" ht="161.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="5"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="6"/>
+      <c r="A36" s="6"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="4"/>
       <c r="E36" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="G36" s="4"/>
+      <c r="G36" s="5"/>
     </row>
     <row r="37" spans="1:7" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="5"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="6" t="s">
+      <c r="A37" s="6"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="4" t="s">
         <v>81</v>
       </c>
       <c r="E37" s="3" t="s">
@@ -1738,104 +1916,104 @@
       <c r="F37" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="G37" s="4"/>
+      <c r="G37" s="5"/>
     </row>
     <row r="38" spans="1:7" ht="171.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="5"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="6"/>
+      <c r="A38" s="6"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="4"/>
       <c r="E38" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="G38" s="4"/>
+      <c r="G38" s="5"/>
     </row>
     <row r="39" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A39" s="5"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="6"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="4"/>
       <c r="E39" s="3" t="s">
         <v>85</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="G39" s="4"/>
+      <c r="G39" s="5"/>
     </row>
     <row r="40" spans="1:7" ht="140.4" x14ac:dyDescent="0.3">
-      <c r="A40" s="5"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="6"/>
+      <c r="A40" s="6"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="4"/>
       <c r="E40" s="2" t="s">
         <v>61</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="G40" s="4"/>
+      <c r="G40" s="5"/>
     </row>
     <row r="41" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A41" s="5"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="6"/>
+      <c r="A41" s="6"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="4"/>
       <c r="E41" s="3" t="s">
         <v>75</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G41" s="4"/>
+      <c r="G41" s="5"/>
     </row>
     <row r="42" spans="1:7" ht="140.4" x14ac:dyDescent="0.3">
-      <c r="A42" s="5"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="6"/>
+      <c r="A42" s="6"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="4"/>
       <c r="E42" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="G42" s="4"/>
+      <c r="G42" s="5"/>
     </row>
     <row r="43" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A43" s="5"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="6"/>
+      <c r="A43" s="6"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="4"/>
       <c r="E43" s="3" t="s">
         <v>77</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G43" s="4"/>
+      <c r="G43" s="5"/>
     </row>
     <row r="44" spans="1:7" ht="171.6" x14ac:dyDescent="0.3">
-      <c r="A44" s="5"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="6"/>
+      <c r="A44" s="6"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="4"/>
       <c r="E44" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="G44" s="4"/>
+      <c r="G44" s="5"/>
     </row>
     <row r="45" spans="1:7" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="5"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="6" t="s">
+      <c r="A45" s="6"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="4" t="s">
         <v>88</v>
       </c>
       <c r="E45" s="3" t="s">
@@ -1844,108 +2022,279 @@
       <c r="F45" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="G45" s="4"/>
+      <c r="G45" s="5"/>
     </row>
     <row r="46" spans="1:7" ht="171.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="5"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="6"/>
+      <c r="A46" s="6"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="4"/>
       <c r="E46" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="G46" s="4"/>
+      <c r="G46" s="5"/>
     </row>
     <row r="47" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A47" s="5"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="6"/>
+      <c r="A47" s="6"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="4"/>
       <c r="E47" s="3" t="s">
         <v>92</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="G47" s="4"/>
+      <c r="G47" s="5"/>
     </row>
     <row r="48" spans="1:7" ht="140.4" x14ac:dyDescent="0.3">
-      <c r="A48" s="5"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="6"/>
+      <c r="A48" s="6"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="4"/>
       <c r="E48" s="2" t="s">
         <v>61</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="G48" s="4"/>
+      <c r="G48" s="5"/>
     </row>
     <row r="49" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A49" s="5"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="6"/>
+      <c r="A49" s="6"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="4"/>
       <c r="E49" s="3" t="s">
         <v>75</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G49" s="4"/>
+      <c r="G49" s="5"/>
     </row>
     <row r="50" spans="1:7" ht="140.4" x14ac:dyDescent="0.3">
-      <c r="A50" s="5"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="6"/>
+      <c r="A50" s="6"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="4"/>
       <c r="E50" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="G50" s="4"/>
+      <c r="G50" s="5"/>
     </row>
     <row r="51" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A51" s="5"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="6"/>
+      <c r="A51" s="6"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="4"/>
       <c r="E51" s="3" t="s">
         <v>77</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G51" s="4"/>
+      <c r="G51" s="5"/>
     </row>
     <row r="52" spans="1:7" ht="171.6" x14ac:dyDescent="0.3">
-      <c r="A52" s="5"/>
-      <c r="B52" s="6"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="6"/>
+      <c r="A52" s="6"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="4"/>
       <c r="E52" s="2" t="s">
         <v>79</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="G52" s="4"/>
+      <c r="G52" s="5"/>
+    </row>
+    <row r="53" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A53" s="9">
+        <v>8</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G53" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="179.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="9"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G54" s="11"/>
+    </row>
+    <row r="55" spans="1:7" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="9">
+        <v>9</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G55" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="156" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="9"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G56" s="11"/>
+    </row>
+    <row r="57" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A57" s="9">
+        <v>10</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="171.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="9"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G58" s="5"/>
+    </row>
+    <row r="59" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A59" s="9">
+        <v>11</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="A60" s="9"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G60" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="D29:D36"/>
-    <mergeCell ref="D37:D44"/>
-    <mergeCell ref="D45:D52"/>
-    <mergeCell ref="G29:G52"/>
-    <mergeCell ref="A29:A52"/>
-    <mergeCell ref="B29:B52"/>
-    <mergeCell ref="C29:C52"/>
+  <mergeCells count="57">
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="B23:B28"/>
+    <mergeCell ref="C23:C28"/>
+    <mergeCell ref="D23:D28"/>
+    <mergeCell ref="G23:G28"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G6:G18"/>
+    <mergeCell ref="G4:G5"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
@@ -1962,20 +2311,13 @@
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G6:G18"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="B23:B28"/>
-    <mergeCell ref="C23:C28"/>
-    <mergeCell ref="D23:D28"/>
-    <mergeCell ref="G23:G28"/>
+    <mergeCell ref="D29:D36"/>
+    <mergeCell ref="D37:D44"/>
+    <mergeCell ref="D45:D52"/>
+    <mergeCell ref="G29:G52"/>
+    <mergeCell ref="A29:A52"/>
+    <mergeCell ref="B29:B52"/>
+    <mergeCell ref="C29:C52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>